<commit_message>
new file creater for sort and filter
</commit_message>
<xml_diff>
--- a/sort_filter.xlsx
+++ b/sort_filter.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DA-9\day-11\sort_filter\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD49F461-8E90-4B36-97FE-2A091383B07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,53 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+  <si>
+    <t>Vegitables</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>potato</t>
+  </si>
+  <si>
+    <t>Cabage</t>
+  </si>
+  <si>
+    <t>Paper</t>
+  </si>
+  <si>
+    <t>Onion</t>
+  </si>
+  <si>
+    <t>Lady Finger</t>
+  </si>
+  <si>
+    <t>Dhaniya</t>
+  </si>
+  <si>
+    <t>D-Shop</t>
+  </si>
+  <si>
+    <t>D-mart</t>
+  </si>
+  <si>
+    <t>C-Shop</t>
+  </si>
+  <si>
+    <t>A-Shop</t>
+  </si>
+  <si>
+    <t>Reliance</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +78,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +116,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +418,208 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C4:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="115" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>35</v>
+      </c>
+      <c r="F5">
+        <v>25</v>
+      </c>
+      <c r="G5">
+        <v>17</v>
+      </c>
+      <c r="H5">
+        <v>28</v>
+      </c>
+      <c r="I5">
+        <v>38</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>25</v>
+      </c>
+      <c r="I6">
+        <v>50</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>180</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>16</v>
+      </c>
+      <c r="H7">
+        <v>22</v>
+      </c>
+      <c r="I7">
+        <v>35</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>150</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>23</v>
+      </c>
+      <c r="I8">
+        <v>35</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>200</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+      <c r="I9">
+        <v>30</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter whole number between 40 to 220_x000a_" sqref="D6" xr:uid="{CE9A4FEF-2021-47CF-8F66-96662F2CC948}">
+      <formula1>40</formula1>
+      <formula2>220</formula2>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter whole number between 40 to 220_x000a_" sqref="D5" xr:uid="{C747562D-F256-459D-B37F-57552FA3D692}">
+      <formula1>40</formula1>
+      <formula2>220</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D9" xr:uid="{1B257330-61DC-4EAD-9926-2131876AD335}">
+      <formula1>50</formula1>
+      <formula2>180</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4" xr:uid="{ED793961-2BB4-4F9D-AB42-DDCED4060D82}">
+      <formula1>40</formula1>
+      <formula2>220</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>